<commit_message>
Played With Laser Calculations
</commit_message>
<xml_diff>
--- a/CougSat1/CougSat1-PayloadCalculations.xlsx
+++ b/CougSat1/CougSat1-PayloadCalculations.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\CougsInSpace\CougSat1-Hardware\CougSat1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BF2C68-2093-4B04-B458-50AB9966C2D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,13 +19,20 @@
     <sheet name="LEDs" sheetId="10" r:id="rId4"/>
     <sheet name="Laser" sheetId="11" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <fileRecoveryPr autoRecover="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="109">
   <si>
     <t>Ground Camera</t>
   </si>
@@ -345,44 +353,51 @@
   </si>
   <si>
     <t>Telescope Aperture Diameter</t>
+  </si>
+  <si>
+    <t>Bits per byte</t>
+  </si>
+  <si>
+    <t>10b/8b encoding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="31">
+  <numFmts count="32">
     <numFmt numFmtId="164" formatCode="0\ &quot;km&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0\ &quot;Cd&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00\ &quot;W&quot;"/>
     <numFmt numFmtId="167" formatCode="0\ &quot;W&quot;"/>
     <numFmt numFmtId="168" formatCode="0\ &quot;sec&quot;"/>
-    <numFmt numFmtId="170" formatCode="0.00E+0\ &quot;lux&quot;"/>
-    <numFmt numFmtId="171" formatCode="0.0\ &quot;°&quot;"/>
-    <numFmt numFmtId="172" formatCode="0\ &quot;Wm⁻²&quot;"/>
-    <numFmt numFmtId="173" formatCode="0\ &quot;lmW⁻¹&quot;"/>
-    <numFmt numFmtId="174" formatCode="&quot;f/&quot;0.0"/>
-    <numFmt numFmtId="175" formatCode="0.00\ &quot;V lux⁻¹ s⁻¹&quot;"/>
-    <numFmt numFmtId="176" formatCode="0.0\ &quot;µs&quot;"/>
-    <numFmt numFmtId="177" formatCode="0.00\ &quot;V&quot;"/>
-    <numFmt numFmtId="178" formatCode="0.00\ &quot;lux s&quot;"/>
-    <numFmt numFmtId="179" formatCode="0.0\ &quot;mm&quot;"/>
-    <numFmt numFmtId="180" formatCode="0.00\ &quot;mm&quot;"/>
-    <numFmt numFmtId="181" formatCode="0\ &quot;px&quot;"/>
-    <numFmt numFmtId="182" formatCode="0\ &quot;m&quot;"/>
-    <numFmt numFmtId="183" formatCode="0\ &quot;mW&quot;"/>
-    <numFmt numFmtId="184" formatCode="0\ &quot;nm&quot;"/>
-    <numFmt numFmtId="185" formatCode="0.00E+0\ &quot;Wm⁻²&quot;"/>
-    <numFmt numFmtId="186" formatCode="0\ &quot;mm&quot;"/>
-    <numFmt numFmtId="187" formatCode="0.00\ &quot;AW⁻¹&quot;"/>
-    <numFmt numFmtId="188" formatCode="0.0\ &quot;dB&quot;"/>
-    <numFmt numFmtId="189" formatCode="0.0"/>
-    <numFmt numFmtId="190" formatCode="0.00E+0\ &quot;W&quot;"/>
-    <numFmt numFmtId="191" formatCode="0.0\ &quot;km&quot;"/>
-    <numFmt numFmtId="192" formatCode="0.0\ &quot;pA&quot;"/>
-    <numFmt numFmtId="193" formatCode="0.0E+0"/>
-    <numFmt numFmtId="194" formatCode="0\ &quot;B&quot;"/>
-    <numFmt numFmtId="200" formatCode="0.0\ &quot;LEDs&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.00E+0\ &quot;lux&quot;"/>
+    <numFmt numFmtId="170" formatCode="0.0\ &quot;°&quot;"/>
+    <numFmt numFmtId="171" formatCode="0\ &quot;Wm⁻²&quot;"/>
+    <numFmt numFmtId="172" formatCode="0\ &quot;lmW⁻¹&quot;"/>
+    <numFmt numFmtId="173" formatCode="&quot;f/&quot;0.0"/>
+    <numFmt numFmtId="174" formatCode="0.00\ &quot;V lux⁻¹ s⁻¹&quot;"/>
+    <numFmt numFmtId="175" formatCode="0.0\ &quot;µs&quot;"/>
+    <numFmt numFmtId="176" formatCode="0.00\ &quot;V&quot;"/>
+    <numFmt numFmtId="177" formatCode="0.00\ &quot;lux s&quot;"/>
+    <numFmt numFmtId="178" formatCode="0.0\ &quot;mm&quot;"/>
+    <numFmt numFmtId="179" formatCode="0.00\ &quot;mm&quot;"/>
+    <numFmt numFmtId="180" formatCode="0\ &quot;px&quot;"/>
+    <numFmt numFmtId="181" formatCode="0\ &quot;m&quot;"/>
+    <numFmt numFmtId="182" formatCode="0\ &quot;mW&quot;"/>
+    <numFmt numFmtId="183" formatCode="0\ &quot;nm&quot;"/>
+    <numFmt numFmtId="184" formatCode="0.00E+0\ &quot;Wm⁻²&quot;"/>
+    <numFmt numFmtId="185" formatCode="0\ &quot;mm&quot;"/>
+    <numFmt numFmtId="186" formatCode="0.00\ &quot;AW⁻¹&quot;"/>
+    <numFmt numFmtId="187" formatCode="0.0\ &quot;dB&quot;"/>
+    <numFmt numFmtId="188" formatCode="0.0"/>
+    <numFmt numFmtId="189" formatCode="0.00E+0\ &quot;W&quot;"/>
+    <numFmt numFmtId="190" formatCode="0.0\ &quot;km&quot;"/>
+    <numFmt numFmtId="191" formatCode="0.0\ &quot;pA&quot;"/>
+    <numFmt numFmtId="192" formatCode="0.0E+0"/>
+    <numFmt numFmtId="193" formatCode="0\ &quot;B&quot;"/>
+    <numFmt numFmtId="194" formatCode="0.0\ &quot;LEDs&quot;"/>
+    <numFmt numFmtId="195" formatCode="0\ &quot;b&quot;"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -549,7 +564,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -567,44 +582,47 @@
     <xf numFmtId="168" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="7" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="174" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="7" fillId="4" borderId="3" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="7" fillId="4" borderId="3" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="7" fillId="4" borderId="3" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="183" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="184" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="185" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="185" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="186" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="187" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="188" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="189" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="190" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="191" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="191" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="192" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="192" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="193" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="193" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="194" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -620,9 +638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="194" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="200" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -1014,25 +1030,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -1040,11 +1056,11 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -1085,23 +1101,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1410,24 +1426,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1456,21 +1472,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1577,7 +1593,7 @@
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="62">
+      <c r="B10" s="57">
         <f>B7/B8</f>
         <v>1.3158507308233127</v>
       </c>
@@ -1650,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF8DECF-9A6D-4CC2-9E9D-6FB05AFCB09B}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,20 +1684,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
@@ -1721,7 +1737,7 @@
         <v>105</v>
       </c>
       <c r="B6" s="31">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>21</v>
@@ -1735,7 +1751,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="9">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>22</v>
@@ -1764,7 +1780,7 @@
       </c>
       <c r="B9" s="41">
         <f>6371*(SQRT((B7+6371)^2/6371^2-COS(RADIANS(B8))^2)-SIN(RADIANS(B8)))</f>
-        <v>739.31977293225555</v>
+        <v>1075.0880169291183</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>24</v>
@@ -1779,7 +1795,7 @@
       </c>
       <c r="B10" s="51">
         <f>TAN(RADIANS(B6))*B9</f>
-        <v>12.904874639247602</v>
+        <v>9.3821509871694637</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>25</v>
@@ -1794,7 +1810,7 @@
       </c>
       <c r="B11" s="44">
         <f>B4/1000/(PI()*(B10*1000)^2)</f>
-        <v>1.9113602380969471E-9</v>
+        <v>3.6161404643885772E-9</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>28</v>
@@ -1840,7 +1856,7 @@
       </c>
       <c r="B14" s="50">
         <f>PI()*(B13/2000)^2*B11*B12</f>
-        <v>1.3240397197623662E-10</v>
+        <v>2.5049770899584621E-10</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>27</v>
@@ -1895,7 +1911,7 @@
       </c>
       <c r="B19" s="53">
         <f>B15*B14*10^12+B16</f>
-        <v>53.961588790494652</v>
+        <v>101.19908359833849</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1904,7 +1920,7 @@
       </c>
       <c r="B20" s="47">
         <f>10*LOG(B19/MAX(B16,B17),10)</f>
-        <v>17.320847281160034</v>
+        <v>20.051765797964013</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1913,7 +1929,7 @@
       </c>
       <c r="B21" s="47">
         <f>10*LOG(B19/MAX(B16,B18),10)</f>
-        <v>17.320847281160034</v>
+        <v>20.051765797964013</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1922,7 +1938,7 @@
       </c>
       <c r="B22" s="54">
         <f>ERFC(SQRT(B19/MAX(B16,B17))/2)/2</f>
-        <v>1.0274354645976482E-7</v>
+        <v>5.6635741705619638E-13</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1931,70 +1947,81 @@
       </c>
       <c r="B23" s="54">
         <f>ERFC(SQRT(B19/MAX(B16,B18))/2)/2</f>
-        <v>1.0274354645976482E-7</v>
+        <v>5.6635741705619638E-13</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="60">
-        <v>1000</v>
+      <c r="B24" s="55">
+        <v>1024</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="B25" s="61">
-        <f>1-(1-B22)^(B24*8)</f>
-        <v>8.2161070690123239E-4</v>
+        <v>107</v>
+      </c>
+      <c r="B25" s="63">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="56">
+        <f>1-(1-B22)^(B24*B25)</f>
+        <v>5.7991655921796337E-9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="61">
-        <f>1-(1-B23)^(B24*8)</f>
-        <v>8.2161070690123239E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="56">
+        <f>1-(1-B23)^(B24*B25)</f>
+        <v>5.7991655921796337E-9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B28" s="21">
         <f>683*10^(-1)</f>
         <v>68.3</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="48">
-        <f>B11*B27</f>
-        <v>1.3054590426202147E-7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="48">
+        <f>B11*B28</f>
+        <v>2.4698239371773983E-7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="49">
-        <f>-14.18-LOG(B28,10)*2.5</f>
-        <v>3.0305918728792349</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B30" s="49">
+        <f>-14.18-LOG(B29,10)*2.5</f>
+        <v>2.3383350114233217</v>
+      </c>
+      <c r="C30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>